<commit_message>
MENAMBAHKAN +62 PADA MENU SISWA
</commit_message>
<xml_diff>
--- a/data_beasiswa.xlsx
+++ b/data_beasiswa.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,7 +454,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ahmad Maulidun</t>
+          <t xml:space="preserve">Ahmad Maulidun </t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -464,7 +464,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Compreng</t>
+          <t>Subang</t>
         </is>
       </c>
     </row>
@@ -509,6 +509,28 @@
       <c r="D4" t="inlineStr">
         <is>
           <t>Cianjur</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>00900980</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Ghisya Adi</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>11221111111</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Subang</t>
         </is>
       </c>
     </row>
@@ -630,11 +652,11 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Habis</t>
+          <t>Tersedia</t>
         </is>
       </c>
     </row>
@@ -679,6 +701,59 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>NISN</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Kode Beasiswa</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Tanggal</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>0098765432</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>B03001</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -705,24 +780,24 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Tanggal</t>
+          <t>Tanggal Pencabutan</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0098765432</t>
+          <t>0012345678</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>B03001</t>
+          <t>B01001</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-27</t>
         </is>
       </c>
     </row>
@@ -739,60 +814,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>NISN</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Kode Beasiswa</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Tanggal Pencabutan</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>0012345678</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>B01001</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Menambahkan sebuah komentar pada masing masing fitur agar dapat mudah di pahami
</commit_message>
<xml_diff>
--- a/data_beasiswa.xlsx
+++ b/data_beasiswa.xlsx
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -706,7 +706,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -745,6 +745,23 @@
       <c r="C2" t="inlineStr">
         <is>
           <t>2025-11-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>0012345678</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B01001</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2025-12-01</t>
         </is>
       </c>
     </row>

</xml_diff>